<commit_message>
Excel updated - unique users added
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel_Data/Epro.xlsx
+++ b/src/test/resources/Excel_Data/Epro.xlsx
@@ -1,37 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chetan.patel\Workspace_rework\work\CucumberEspire\src\test\resources\Excel_Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A878DC04-C104-4DD4-891C-4012D7AB53DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13830" windowHeight="4430"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Epro_details" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
   <si>
     <t>UserName</t>
   </si>
@@ -213,9 +207,6 @@
     <t>Automated_Campaign_8</t>
   </si>
   <si>
-    <t>Password@123457</t>
-  </si>
-  <si>
     <t>Paper_cost</t>
   </si>
   <si>
@@ -223,13 +214,37 @@
   </si>
   <si>
     <t>Estimate_Reference_number</t>
+  </si>
+  <si>
+    <t>Staginguser_35</t>
+  </si>
+  <si>
+    <t>Staginguser_36</t>
+  </si>
+  <si>
+    <t>Staginguser_37</t>
+  </si>
+  <si>
+    <t>Staginguser_38</t>
+  </si>
+  <si>
+    <t>Staginguser_39</t>
+  </si>
+  <si>
+    <t>Staginguser_15</t>
+  </si>
+  <si>
+    <t>Staginguser_16</t>
+  </si>
+  <si>
+    <t>Staginguser_17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -610,30 +625,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.25" customWidth="1"/>
-    <col min="2" max="2" width="19.25" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" customWidth="1"/>
-    <col min="5" max="5" width="22.08203125" customWidth="1"/>
-    <col min="6" max="6" width="21.25" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="10" max="10" width="25.6640625" customWidth="1"/>
-    <col min="11" max="11" width="26.5" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" customWidth="1"/>
-    <col min="14" max="14" width="13.75" customWidth="1"/>
+    <col min="1" max="1" width="18.90625" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" customWidth="1"/>
+    <col min="3" max="3" width="24.6328125" customWidth="1"/>
+    <col min="4" max="4" width="26.1796875" customWidth="1"/>
+    <col min="5" max="5" width="22.08984375" customWidth="1"/>
+    <col min="6" max="6" width="21.26953125" customWidth="1"/>
+    <col min="7" max="7" width="23.6328125" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" customWidth="1"/>
+    <col min="10" max="10" width="25.6328125" customWidth="1"/>
+    <col min="11" max="11" width="26.453125" customWidth="1"/>
+    <col min="13" max="13" width="16.36328125" customWidth="1"/>
+    <col min="14" max="14" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -665,19 +680,19 @@
         <v>17</v>
       </c>
       <c r="K1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L1" t="s">
         <v>18</v>
       </c>
       <c r="M1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N1" t="s">
         <v>61</v>
       </c>
-      <c r="N1" t="s">
-        <v>62</v>
-      </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -721,9 +736,9 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -765,9 +780,9 @@
         <v>231</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -809,12 +824,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
         <v>55</v>
@@ -853,9 +868,9 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -897,9 +912,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -941,12 +956,12 @@
         <v>312</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
         <v>58</v>
@@ -985,9 +1000,9 @@
         <v>312</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
@@ -1027,21 +1042,156 @@
       </c>
       <c r="N9">
         <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10">
+        <v>123</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>435</v>
+      </c>
+      <c r="J10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10">
+        <v>45</v>
+      </c>
+      <c r="M10">
+        <v>123</v>
+      </c>
+      <c r="N10">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11">
+        <v>123</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>435</v>
+      </c>
+      <c r="J11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11">
+        <v>45</v>
+      </c>
+      <c r="M11">
+        <v>123</v>
+      </c>
+      <c r="N11">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12">
+        <v>123</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>435</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12">
+        <v>45</v>
+      </c>
+      <c r="M12">
+        <v>123</v>
+      </c>
+      <c r="N12">
+        <v>312</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4" display="Password@123456"/>
-    <hyperlink ref="B8" r:id="rId5"/>
-    <hyperlink ref="B6" r:id="rId6"/>
-    <hyperlink ref="B9" r:id="rId7"/>
-    <hyperlink ref="B7" r:id="rId8"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{9657C0D8-AE00-418F-A3CB-8E644357B0D9}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{75EA1695-F298-4051-8F54-12F345F62960}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{35535ABC-9DC3-49F7-A0AB-6107432CBB2D}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{72F622C0-F3C3-41C2-8D96-F3A0A3D8E981}"/>
+    <hyperlink ref="B5" r:id="rId11" xr:uid="{2E898877-AD65-4671-954F-DD1D1AA80F8F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>